<commit_message>
seperated new companies in diffirent file
</commit_message>
<xml_diff>
--- a/NEWLY LISTED.xlsx
+++ b/NEWLY LISTED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neerajkumar/stockanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B13D13-8006-6C4F-B220-E001DACD1878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C4B01-8BB3-154E-A59A-C16833BD6F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="26740" windowHeight="14860" xr2:uid="{50A91AAF-87EE-1B48-9504-F3E1AB3628A0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{50A91AAF-87EE-1B48-9504-F3E1AB3628A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>SYMBOL</t>
   </si>
@@ -49,6 +49,63 @@
   </si>
   <si>
     <t>TATVA</t>
+  </si>
+  <si>
+    <t>NYKAA</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>CAMS</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>CLEAN</t>
+  </si>
+  <si>
+    <t>RITES</t>
+  </si>
+  <si>
+    <t>ZOMOTO</t>
+  </si>
+  <si>
+    <t>NUVOCO</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>LXCHEM</t>
+  </si>
+  <si>
+    <t>EASEMYTRIP-BE</t>
+  </si>
+  <si>
+    <t>IPL</t>
+  </si>
+  <si>
+    <t>ROSSARI</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>UTIAMC</t>
+  </si>
+  <si>
+    <t>CHEMCON</t>
+  </si>
+  <si>
+    <t>HAPPSTMNDS-BE</t>
+  </si>
+  <si>
+    <t>IEX</t>
+  </si>
+  <si>
+    <t>CRAFTSMAN</t>
   </si>
 </sst>
 </file>
@@ -400,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE596D-4935-334E-868D-CD5EEA50642D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,6 +493,126 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>